<commit_message>
mz: fixed sql lite link issue.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Mozambique/November 2021/mz_lf_pretas_1_site_202111.xlsx
+++ b/LF/PreTAS/Mozambique/November 2021/mz_lf_pretas_1_site_202111.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="349">
   <si>
     <t>type</t>
   </si>
@@ -66,6 +66,36 @@
     <t>choice_filter</t>
   </si>
   <si>
+    <t>select_one recorder_list</t>
+  </si>
+  <si>
+    <t>c_recorder</t>
+  </si>
+  <si>
+    <t>Enter Recorder ID</t>
+  </si>
+  <si>
+    <t>If you are the only recorder on your team, this may be called a "team ID". Recorder ID is the 2-digit code assigned to you or your team.</t>
+  </si>
+  <si>
+    <t>Insira o código do gravador</t>
+  </si>
+  <si>
+    <t>Se você for o único registrador/inqueridor na sua equipe, isso pode ser chamado de "ID de equipe". ID do inqueridor é o código de 2 dígitos fornecido a você ou à sua equipe.</t>
+  </si>
+  <si>
+    <t>regex(.,'^[0-9]{2}$')</t>
+  </si>
+  <si>
+    <t>The code must be a two-digit number between 9 and 100</t>
+  </si>
+  <si>
+    <t>O código deve ser um número de dois dígitos entre 9 e 100</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>select_one eu_list</t>
   </si>
   <si>
@@ -78,51 +108,21 @@
     <t>Selecione o Província</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>select_one recorder_list</t>
-  </si>
-  <si>
-    <t>c_recorder</t>
-  </si>
-  <si>
-    <t>Enter Recorder ID</t>
-  </si>
-  <si>
-    <t>If you are the only recorder on your team, this may be called a "team ID". Recorder ID is the 2-digit code assigned to you or your team.</t>
-  </si>
-  <si>
-    <t>Insira o código do gravador</t>
-  </si>
-  <si>
-    <t>Se você for o único registrador/inqueridor na sua equipe, isso pode ser chamado de "ID de equipe". ID do inqueridor é o código de 2 dígitos fornecido a você ou à sua equipe.</t>
-  </si>
-  <si>
-    <t>regex(.,'^[0-9]{2}$')</t>
-  </si>
-  <si>
-    <t>The code must be a two-digit number between 9 and 100</t>
-  </si>
-  <si>
-    <t>O código deve ser um número de dois dígitos entre 9 e 100</t>
+    <t>select_one district_list</t>
+  </si>
+  <si>
+    <t>c_district</t>
+  </si>
+  <si>
+    <t>Select your district</t>
+  </si>
+  <si>
+    <t>Selecione o distrito</t>
   </si>
   <si>
     <t>eu_list = ${c_province}</t>
   </si>
   <si>
-    <t>select_one district_list</t>
-  </si>
-  <si>
-    <t>c_district</t>
-  </si>
-  <si>
-    <t>Select your district</t>
-  </si>
-  <si>
-    <t>Selecione o distrito</t>
-  </si>
-  <si>
     <t>select_one site_names</t>
   </si>
   <si>
@@ -1056,10 +1056,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Nov 2021) Pre-TAS FL - 1. Conglomerado V2.1</t>
-  </si>
-  <si>
-    <t>mz_lf_pretas_1_site_202111_v2_1</t>
+    <t>(Nov 2021) Pre-TAS FL - 1. Conglomerado V2.2</t>
+  </si>
+  <si>
+    <t>mz_lf_pretas_1_site_202111_v2_2</t>
   </si>
   <si>
     <t>Portuguese</t>
@@ -1115,14 +1115,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1136,15 +1128,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1152,38 +1137,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1197,7 +1159,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1208,6 +1170,14 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1226,8 +1196,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1241,26 +1227,40 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1297,7 +1297,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1309,43 +1315,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1363,7 +1333,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1375,7 +1399,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1387,19 +1411,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1411,67 +1453,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1510,30 +1510,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1559,11 +1535,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1583,165 +1565,183 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2165,7 +2165,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -2237,7 +2237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" spans="1:16">
+    <row r="2" s="3" customFormat="1" ht="42.75" spans="1:16">
       <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
@@ -2247,77 +2247,75 @@
       <c r="C2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="24" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="23"/>
-    </row>
-    <row r="3" s="3" customFormat="1" ht="42.75" spans="1:16">
+        <v>25</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" s="3" customFormat="1" spans="1:16">
       <c r="A3" s="23" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>24</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D3" s="24"/>
       <c r="E3" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="23"/>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:16">
       <c r="A4" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="24" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>33</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="10"/>
@@ -2327,12 +2325,12 @@
       <c r="K4" s="23"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:16">
@@ -2361,7 +2359,7 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
@@ -2391,7 +2389,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
@@ -2421,7 +2419,7 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -2449,7 +2447,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
@@ -2479,7 +2477,7 @@
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
@@ -2513,7 +2511,7 @@
       </c>
       <c r="L10" s="23"/>
       <c r="M10" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>

</xml_diff>